<commit_message>
fix temperature legend in figures appendix 15th -april
</commit_message>
<xml_diff>
--- a/stats/general/table_general.xlsx
+++ b/stats/general/table_general.xlsx
@@ -1,97 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s2096910_ed_ac_uk/Documents/dissertation/dissertation/dissertation/stats/general/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_AABA903B1DB166A9A2D62A493F9B0E619259AA3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42F7F611-A61E-014A-92B4-87BE17FD9F09}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13120" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austroplaca_X3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryum_X1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryum_X2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryum_X4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bryum_average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total active hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% active hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Thallus temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min Thallus temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max Thallus temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Thallus temp active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min Thallus temp active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max Thallus temp active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max Par</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX Yield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yield</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max ETR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean air T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min air T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max air T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RH (%)</t>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Austroplaca_X3</t>
+  </si>
+  <si>
+    <t>Bryum_X1</t>
+  </si>
+  <si>
+    <t>Bryum_X2</t>
+  </si>
+  <si>
+    <t>Bryum_X4</t>
+  </si>
+  <si>
+    <t>Bryum_average</t>
+  </si>
+  <si>
+    <t>Total active hours</t>
+  </si>
+  <si>
+    <t>% active hours</t>
+  </si>
+  <si>
+    <t>Average Thallus temp</t>
+  </si>
+  <si>
+    <t>Min Thallus temp</t>
+  </si>
+  <si>
+    <t>Max Thallus temp</t>
+  </si>
+  <si>
+    <t>Average Thallus temp active</t>
+  </si>
+  <si>
+    <t>Min Thallus temp active</t>
+  </si>
+  <si>
+    <t>Max Thallus temp active</t>
+  </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>Max Par</t>
+  </si>
+  <si>
+    <t>MAX Yield</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>ETR</t>
+  </si>
+  <si>
+    <t>Max ETR</t>
+  </si>
+  <si>
+    <t>mean air T</t>
+  </si>
+  <si>
+    <t>min air T</t>
+  </si>
+  <si>
+    <t>max air T</t>
+  </si>
+  <si>
+    <t>RH (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -127,6 +147,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,14 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,368 +466,440 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>4992</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>4633</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>4165</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>4810</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>4380</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="G2">
+        <f>STDEV(C2:E2)</f>
+        <v>333.26115885293325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>11.7744180012737</v>
       </c>
-      <c r="C3" t="n">
-        <v>10.9286910574859</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9.82473521571958</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C3">
+        <v>10.928691057485899</v>
+      </c>
+      <c r="D3">
+        <v>9.8247352157195795</v>
+      </c>
+      <c r="E3">
         <v>11.3462128181539</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>10.331894416531</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="G3">
+        <f t="shared" ref="G3:G19" si="0">STDEV(C3:E3)</f>
+        <v>0.7861230836527846</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>-16.6858231311775</v>
       </c>
-      <c r="C4" t="n">
-        <v>-15.796933455995</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>-15.796933455994999</v>
+      </c>
+      <c r="D4">
         <v>-16.2554289623282</v>
       </c>
-      <c r="E4" t="n">
-        <v>-16.441719151747</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-16.441719151747</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="E4">
+        <v>-16.441719151747002</v>
+      </c>
+      <c r="F4">
+        <v>-16.441719151747002</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.331830970386989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>-31.7</v>
       </c>
-      <c r="C5" t="n">
-        <v>-32.2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-33.2</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="C5">
+        <v>-32.200000000000003</v>
+      </c>
+      <c r="D5">
+        <v>-33.200000000000003</v>
+      </c>
+      <c r="E5">
         <v>-32.4</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>-32.6</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.52915026221291894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>14.8</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>15</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>10.8</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>13.3</v>
       </c>
-      <c r="F6" t="n">
-        <v>13.0333333333333</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="F6">
+        <v>13.033333333333299</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.1126602503320977</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.271709076337396</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7">
+        <v>0.27170907633739599</v>
+      </c>
+      <c r="C7">
         <v>1.55823440535289</v>
       </c>
-      <c r="D7" t="n">
-        <v>0.955270108043219</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.718149688149689</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="D7">
+        <v>0.95527010804321899</v>
+      </c>
+      <c r="E7">
+        <v>0.71814968814968905</v>
+      </c>
+      <c r="F7">
         <v>1.07721806718193</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0.43311552912954826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>-7.9</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>-6.7</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>-5.4</v>
       </c>
-      <c r="E8" t="n">
-        <v>-8.2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-6.76666666666667</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="E8">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="F8">
+        <v>-6.7666666666666702</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1.4011899704655819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>12.8</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>15</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>10.5</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>12.8</v>
       </c>
-      <c r="F9" t="n">
-        <v>12.7666666666667</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="F9">
+        <v>12.766666666666699</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.250185177565029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>175.083750751352</v>
       </c>
-      <c r="C10" t="n">
-        <v>331.049859702138</v>
-      </c>
-      <c r="D10" t="n">
-        <v>368.146458583434</v>
-      </c>
-      <c r="E10" t="n">
-        <v>218.458835758835</v>
-      </c>
-      <c r="F10" t="n">
-        <v>305.885051348136</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="C10">
+        <v>331.04985970213801</v>
+      </c>
+      <c r="D10">
+        <v>368.14645858343403</v>
+      </c>
+      <c r="E10">
+        <v>218.45883575883499</v>
+      </c>
+      <c r="F10">
+        <v>305.88505134813602</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>77.952208380135943</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1360</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1335</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>2116</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>1472</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>1641</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>417.0263780625873</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>0.8</v>
       </c>
-      <c r="C12" t="n">
-        <v>0.532</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.673</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="C12">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="D12">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="E12">
         <v>0.622</v>
       </c>
-      <c r="F12" t="n">
-        <v>0.609</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="F12">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>7.1393276994406132E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="n">
-        <v>0.246332756629333</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.317072523203108</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="B13">
+        <v>0.24633275662933299</v>
+      </c>
+      <c r="C13">
+        <v>0.31707252320310803</v>
+      </c>
+      <c r="D13">
         <v>0.45254693877551</v>
       </c>
-      <c r="E13" t="n">
-        <v>0.311006237006237</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.360208566328285</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="E13">
+        <v>0.31100623700623697</v>
+      </c>
+      <c r="F13">
+        <v>0.36020856632828502</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>8.0024878798454963E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="n">
-        <v>42.2250012949651</v>
-      </c>
-      <c r="C14" t="n">
-        <v>47.0808979063242</v>
-      </c>
-      <c r="D14" t="n">
-        <v>66.8242737094838</v>
-      </c>
-      <c r="E14" t="n">
+      <c r="B14">
+        <v>42.225001294965097</v>
+      </c>
+      <c r="C14">
+        <v>47.080897906324203</v>
+      </c>
+      <c r="D14">
+        <v>66.824273709483805</v>
+      </c>
+      <c r="E14">
         <v>30.2252806652807</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>48.0434840936962</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>18.318474338451232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="n">
-        <v>489.998</v>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15">
+        <v>489.99799999999999</v>
+      </c>
+      <c r="C15">
         <v>206.6</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>404.8</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>170.3</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>260.566666666667</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>126.22148522867779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>